<commit_message>
Addedd Sapphire FPSQ model
</commit_message>
<xml_diff>
--- a/Examples/Experiment/AlN/TestDataBase.xlsx
+++ b/Examples/Experiment/AlN/TestDataBase.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\home\Software\PDielec\Examples\Experiment\AlN\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937F40D9-C4A7-4828-BD66-6E57FFBAC106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="12800" windowHeight="8030"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
-    <sheet name="Silicon" sheetId="2" r:id="rId2"/>
-    <sheet name="6H-SiC" sheetId="3" r:id="rId3"/>
+    <sheet name="Sapphire" sheetId="4" r:id="rId2"/>
+    <sheet name="Silicon" sheetId="2" r:id="rId3"/>
+    <sheet name="6H-SiC" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"6H-SiC"</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Information"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Silicon"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"6H-SiC"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Silicon"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="191029" iterate="1"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>Information</t>
   </si>
@@ -157,46 +164,112 @@
   </si>
   <si>
     <t>Unkown</t>
+  </si>
+  <si>
+    <t>cm-1</t>
+  </si>
+  <si>
+    <t>Microns</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>D . F . Edwards, in Handbook of Optical Constants of Solids, edited by E. D. Palik (Academic, Orlando, 1985), pp. 547-569.</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>epsinf</t>
+  </si>
+  <si>
+    <t>Omega</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>yy</t>
+  </si>
+  <si>
+    <t>Cell information taken from Capitani et al.</t>
+  </si>
+  <si>
+    <t>zz</t>
+  </si>
+  <si>
+    <t>American Minerologist (2007) 92, 403</t>
+  </si>
+  <si>
+    <t>DOI: 10.2138/am.2007.2346</t>
+  </si>
+  <si>
+    <t>W. G. Spitzer, D. Kleinman, and D. Walsh, Phys. Rev. 113, 127 (1959). L. A. Patrick and W. J. Choyke, Phys. Rev. B 2, 2255 (1970)</t>
+  </si>
+  <si>
+    <t>FPSQ</t>
+  </si>
+  <si>
+    <t>M.Schubert, T.E. Tiwlad, C.M. Herzinger, Phys Rev B Vol 61 (2000) 8187</t>
+  </si>
+  <si>
+    <t>Omega TO</t>
+  </si>
+  <si>
+    <t>Omega LO</t>
+  </si>
+  <si>
+    <t>Room Temperature</t>
+  </si>
+  <si>
+    <t>Eps0</t>
+  </si>
+  <si>
+    <t>Gamma TO</t>
+  </si>
+  <si>
+    <t>Gamma LO</t>
+  </si>
+  <si>
+    <t>Cell information taken from Lutterotti and Scardi</t>
+  </si>
+  <si>
+    <t>Journal of Applied Crystallography 1990, 23, 246-252</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt formatCode="0.00000" numFmtId="100"/>
-    <numFmt formatCode="0.000" numFmtId="101"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <vertAlign val="baseline"/>
-      <sz val="11"/>
-      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,113 +281,393 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="2" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:XFD43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" style="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="12.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" ht="15">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" ht="15">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" ht="15">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" ht="15">
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" ht="15">
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" ht="15">
+    <row r="10" spans="1:4">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" ht="15">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" ht="15">
+    <row r="14" spans="1:4">
       <c r="C14" t="s">
         <v>8</v>
       </c>
@@ -322,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" ht="15">
+    <row r="15" spans="1:4">
       <c r="C15" t="s">
         <v>10</v>
       </c>
@@ -330,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" ht="15">
+    <row r="16" spans="1:4">
       <c r="C16" t="s">
         <v>12</v>
       </c>
@@ -338,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16384" ht="15">
+    <row r="17" spans="1:4">
       <c r="C17" t="s">
         <v>13</v>
       </c>
@@ -346,17 +699,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:16384" ht="15">
+    <row r="18" spans="1:4">
       <c r="C18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:16384" ht="15">
+    <row r="19" spans="1:4">
       <c r="C19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:16384" ht="15">
+    <row r="20" spans="1:4">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -365,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16384" ht="15">
+    <row r="21" spans="1:4">
       <c r="C21" t="s">
         <v>17</v>
       </c>
@@ -373,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:16384" ht="15">
+    <row r="22" spans="1:4">
       <c r="C22" t="s">
         <v>19</v>
       </c>
@@ -381,7 +734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:16384" ht="15">
+    <row r="23" spans="1:4">
       <c r="C23" t="s">
         <v>21</v>
       </c>
@@ -389,7 +742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16384" ht="15">
+    <row r="24" spans="1:4">
       <c r="C24" t="s">
         <v>23</v>
       </c>
@@ -397,7 +750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:16384" ht="15">
+    <row r="25" spans="1:4">
       <c r="C25" t="s">
         <v>25</v>
       </c>
@@ -405,7 +758,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:16384" ht="15">
+    <row r="26" spans="1:4">
       <c r="C26" t="s">
         <v>27</v>
       </c>
@@ -413,7 +766,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:16384" ht="15">
+    <row r="27" spans="1:4">
       <c r="C27" t="s">
         <v>29</v>
       </c>
@@ -421,7 +774,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" ht="15">
+    <row r="28" spans="1:4">
       <c r="C28" t="s">
         <v>31</v>
       </c>
@@ -429,7 +782,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:16384" ht="15">
+    <row r="29" spans="1:4">
       <c r="C29" t="s">
         <v>33</v>
       </c>
@@ -437,7 +790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:16384" ht="15">
+    <row r="30" spans="1:4">
       <c r="C30" t="s">
         <v>35</v>
       </c>
@@ -445,90 +798,417 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:16384" ht="15">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:16384" ht="15">
+    <row r="33" spans="1:2">
       <c r="B33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:16384" ht="15">
+    <row r="34" spans="1:2">
       <c r="B34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" ht="15">
+    <row r="35" spans="1:2">
       <c r="B35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:16384" ht="15">
+    <row r="36" spans="1:2">
       <c r="B36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:16384" ht="15">
+    <row r="37" spans="1:2">
       <c r="B37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:16384" ht="15"/>
-    <row r="43" spans="1:16384" ht="15">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4772E1-D662-43D8-9F56-6A109324F2F7}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" ht="15">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2">
+        <v>9.3849999999999998</v>
+      </c>
+      <c r="C2" s="5">
+        <v>384.99</v>
+      </c>
+      <c r="D2" s="5">
+        <v>387.6</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>3.98</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="15">
+      <c r="C3" s="5">
+        <v>439.1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>481.68</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>4.7605000000000004</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="15">
+      <c r="C4" s="6">
+        <v>569</v>
+      </c>
+      <c r="D4" s="5">
+        <v>629.5</v>
+      </c>
+      <c r="E4" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>4.7605000000000004</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="15">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>633.63</v>
+      </c>
+      <c r="D5" s="5">
+        <v>906.6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>14.7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5">
+        <v>12.9956</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="15">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9.3849999999999998</v>
+      </c>
+      <c r="C6" s="5">
+        <v>384.99</v>
+      </c>
+      <c r="D6" s="5">
+        <v>387.6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>90</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="15">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5">
+        <v>439.1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>481.68</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <v>569</v>
+      </c>
+      <c r="D8" s="5">
+        <v>629.5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8">
+        <v>120</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>633.63</v>
+      </c>
+      <c r="D9" s="5">
+        <v>906.6</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>14.7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="15">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="2">
+        <v>11.614000000000001</v>
+      </c>
+      <c r="C10" s="5">
+        <v>397.52</v>
+      </c>
+      <c r="D10" s="5">
+        <v>510.87</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <f>MIN(A5:A621)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="15">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5">
+        <v>582.41</v>
+      </c>
+      <c r="D11" s="5">
+        <v>881.1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <f>MAX(A5:A621)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="15">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <f>COUNT(A5:A621)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="15">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="2" width="12.856370192307693"/>
+    <col min="1" max="16384" width="12.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>cm-1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Microns</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -539,7 +1219,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="C2" s="3">
-        <v>3.4199999999999999</v>
+        <v>3.42</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -549,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>2.3300000000000001</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -591,67 +1271,47 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>D . F . Edwards, in Handbook of Optical Constants of Solids, edited by E. D. Palik (Academic, Orlando, 1985), pp. 547-569.</t>
-        </is>
+      <c r="H7" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" style="2" width="12.856370192307693"/>
-    <col min="8" max="8" style="2" width="9.140625" customWidth="1"/>
-    <col min="9" max="16384" style="2" width="12.856370192307693"/>
+    <col min="1" max="7" width="12.85546875" style="2"/>
+    <col min="8" max="8" width="9.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="12.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Direction</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>epsinf</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Omega</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Strength</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Gamma</t>
-        </is>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -660,17 +1320,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>xx</t>
-        </is>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>54</v>
       </c>
       <c r="B2">
-        <v>6.5199999999999996</v>
+        <v>6.52</v>
       </c>
       <c r="C2" s="3">
-        <v>793.89999999999998</v>
+        <v>793.9</v>
       </c>
       <c r="D2" s="4">
         <v>1423.5608648737152</v>
@@ -682,20 +1340,18 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>2.3300000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>yy</t>
-        </is>
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>55</v>
       </c>
       <c r="B3">
-        <v>6.5199999999999996</v>
+        <v>6.52</v>
       </c>
       <c r="C3" s="3">
-        <v>793.89999999999998</v>
+        <v>793.9</v>
       </c>
       <c r="D3" s="4">
         <v>1423.5608648737152</v>
@@ -709,23 +1365,19 @@
       <c r="H3">
         <v>3.081</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Cell information taken from Capitani et al.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>zz</t>
-        </is>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>57</v>
       </c>
       <c r="B4">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="C4">
-        <v>785.89999999999998</v>
+        <v>785.9</v>
       </c>
       <c r="D4" s="4">
         <v>1427.7213529999999</v>
@@ -739,15 +1391,13 @@
       <c r="H4">
         <v>3.081</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>American Minerologist (2007) 92, 403</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16.5">
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5">
-        <v>882.89999999999998</v>
+        <v>882.9</v>
       </c>
       <c r="D5" s="4">
         <v>243.56066999999999</v>
@@ -761,13 +1411,11 @@
       <c r="H5">
         <v>15.1248</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>DOI: 10.2138/am.2007.2346</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5">
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="G6" t="s">
         <v>31</v>
       </c>
@@ -775,7 +1423,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.5">
+    <row r="7" spans="1:10">
       <c r="G7" t="s">
         <v>33</v>
       </c>
@@ -783,7 +1431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16.5">
+    <row r="8" spans="1:10">
       <c r="G8" t="s">
         <v>35</v>
       </c>
@@ -791,7 +1439,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16.5">
+    <row r="9" spans="1:10">
       <c r="G9" t="s">
         <v>13</v>
       </c>
@@ -799,7 +1447,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.5">
+    <row r="10" spans="1:10">
       <c r="G10" t="s">
         <v>14</v>
       </c>
@@ -808,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16.5">
+    <row r="11" spans="1:10">
       <c r="G11" t="s">
         <v>15</v>
       </c>
@@ -817,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16.5">
+    <row r="12" spans="1:10">
       <c r="G12" t="s">
         <v>16</v>
       </c>
@@ -826,24 +1474,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16.5">
+    <row r="13" spans="1:10">
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>W. G. Spitzer, D. Kleinman, and D. Walsh, Phys. Rev. 113, 127 (1959). L. A. Patrick and W. J. Choyke, Phys. Rev. B 2, 2255 (1970)</t>
-        </is>
+      <c r="H13" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
</xml_diff>